<commit_message>
update the jupyter notebook
Use the re.sub method;
Update the .gitignore;
undate the inv_info_sample.xlsx
</commit_message>
<xml_diff>
--- a/inv_info_sample.xlsx
+++ b/inv_info_sample.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ningchuanpeng/Documents/GitHub/invoice-automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB44A99-6BF0-114A-8CC1-1298D6A06B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7E8363-521D-7942-86F1-9B3FFCA6AAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{F3C95119-47EE-434B-ACFE-389BE8C7694A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16340" xr2:uid="{F3C95119-47EE-434B-ACFE-389BE8C7694A}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="For booking" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">sheet1!$A$1:$I$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">sheet1!$A$1:$J$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="55">
   <si>
     <t>Amount</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>Inv_No</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -226,6 +223,14 @@
   </si>
   <si>
     <t>Product 15</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invoice No.</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -235,7 +240,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -392,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -431,9 +436,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -441,28 +449,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -792,625 +779,684 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA14FFEB-22C8-4B37-B805-3E79E719FB02}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="C2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F2" s="7">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="str">
+        <f>G2 &amp; " details"</f>
+        <v>Product 1 details</v>
+      </c>
+      <c r="I2" s="6">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16">
+      <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F3" s="7">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="5" t="str">
+        <f t="shared" ref="H3:H20" si="0">G3 &amp; " details"</f>
+        <v>Product 2 details</v>
+      </c>
+      <c r="I3" s="6">
+        <v>59</v>
+      </c>
+      <c r="J3" s="7">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16">
-      <c r="A2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="7">
-        <v>30</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="5" t="str">
-        <f>F2 &amp; " details"</f>
-        <v>Product 1 details</v>
-      </c>
-      <c r="H2" s="6">
-        <v>9</v>
-      </c>
-      <c r="I2" s="7">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16">
-      <c r="A3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="7">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F4" s="7">
+        <v>30</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="5" t="str">
-        <f t="shared" ref="G3:G20" si="0">F3 &amp; " details"</f>
-        <v>Product 2 details</v>
-      </c>
-      <c r="H3" s="6">
-        <v>59</v>
-      </c>
-      <c r="I3" s="7">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="16">
-      <c r="A4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="7">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="5" t="str">
+      <c r="H4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 3 details</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>39</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16">
+    <row r="5" spans="1:10" ht="16">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="7">
-        <v>30</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E5" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F5" s="7">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 4 details</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>13</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>526</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16">
+    <row r="6" spans="1:10" ht="16">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="7">
-        <v>30</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E6" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F6" s="7">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 5 details</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>71</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="7">
         <v>695</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16">
+    <row r="7" spans="1:10" ht="16">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="7">
-        <v>30</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E7" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F7" s="7">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 6 details</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>8</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>632</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16">
+    <row r="8" spans="1:10" ht="16">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="7">
-        <v>30</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E8" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F8" s="7">
+        <v>30</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 7 details</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="6">
         <v>69</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16">
+    <row r="9" spans="1:10" ht="16">
       <c r="A9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="7">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E9" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F9" s="7">
+        <v>30</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 8 details</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="6">
         <v>35</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16">
+    <row r="10" spans="1:10" ht="16">
       <c r="A10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="7">
-        <v>30</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E10" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F10" s="7">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 9 details</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="6">
         <v>73</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="16">
+    <row r="11" spans="1:10" ht="16">
       <c r="A11" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="7">
-        <v>30</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E11" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F11" s="7">
+        <v>30</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 10 details</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>23</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16">
+    <row r="12" spans="1:10" ht="16">
       <c r="A12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="7">
-        <v>30</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E12" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F12" s="7">
+        <v>30</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 11 details</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I12" s="6">
         <v>13</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J12" s="7">
         <v>598</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="16">
+    <row r="13" spans="1:10" ht="16">
       <c r="A13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="7">
-        <v>30</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E13" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F13" s="7">
+        <v>30</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 12 details</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="6">
         <v>67</v>
       </c>
-      <c r="I13" s="7">
+      <c r="J13" s="7">
         <v>587</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16">
+    <row r="14" spans="1:10" ht="16">
       <c r="A14" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="7">
-        <v>30</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E14" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F14" s="7">
+        <v>30</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 13 details</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="6">
         <v>70</v>
       </c>
-      <c r="I14" s="7">
+      <c r="J14" s="7">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="16">
+    <row r="15" spans="1:10" ht="16">
       <c r="A15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="7">
-        <v>30</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E15" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F15" s="7">
+        <v>30</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 14 details</v>
       </c>
-      <c r="H15" s="6">
+      <c r="I15" s="6">
         <v>56</v>
       </c>
-      <c r="I15" s="7">
+      <c r="J15" s="7">
         <v>639</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16">
+    <row r="16" spans="1:10" ht="16">
       <c r="A16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="7">
-        <v>30</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="5" t="str">
+        <v>30</v>
+      </c>
+      <c r="E16" s="17">
+        <v>45657</v>
+      </c>
+      <c r="F16" s="7">
+        <v>30</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 15 details</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="6">
         <v>12</v>
       </c>
-      <c r="I16" s="7">
+      <c r="J16" s="7">
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="16">
+    <row r="17" spans="1:10" ht="16">
       <c r="A17" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="7">
+        <v>32</v>
+      </c>
+      <c r="E17" s="17">
+        <v>45668</v>
+      </c>
+      <c r="F17" s="7">
         <v>90</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="5" t="str">
+      <c r="G17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 7 details</v>
       </c>
-      <c r="H17" s="12">
+      <c r="I17" s="12">
         <v>69</v>
       </c>
-      <c r="I17" s="7">
+      <c r="J17" s="7">
         <v>302</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16">
+    <row r="18" spans="1:10" ht="16">
       <c r="A18" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="7">
+        <v>33</v>
+      </c>
+      <c r="E18" s="17">
+        <v>45704</v>
+      </c>
+      <c r="F18" s="7">
         <v>60</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="5" t="str">
+      <c r="G18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 2 details</v>
       </c>
-      <c r="H18" s="12">
+      <c r="I18" s="12">
         <v>59</v>
       </c>
-      <c r="I18" s="7">
+      <c r="J18" s="7">
         <v>598</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="16">
+    <row r="19" spans="1:10" ht="16">
       <c r="A19" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="7">
+        <v>33</v>
+      </c>
+      <c r="E19" s="17">
+        <v>45704</v>
+      </c>
+      <c r="F19" s="7">
         <v>60</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="5" t="str">
+      <c r="G19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 10 details</v>
       </c>
-      <c r="H19" s="12">
+      <c r="I19" s="12">
         <v>23</v>
       </c>
-      <c r="I19" s="7">
+      <c r="J19" s="7">
         <v>463</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16">
+    <row r="20" spans="1:10" ht="16">
       <c r="A20" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="7">
+        <v>33</v>
+      </c>
+      <c r="E20" s="17">
+        <v>45737</v>
+      </c>
+      <c r="F20" s="7">
         <v>60</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="5" t="str">
+      <c r="G20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Product 15 details</v>
       </c>
-      <c r="H20" s="12">
+      <c r="I20" s="12">
         <v>12</v>
       </c>
-      <c r="I20" s="7">
+      <c r="J20" s="7">
         <v>552</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I20" xr:uid="{EA14FFEB-22C8-4B37-B805-3E79E719FB02}"/>
+  <autoFilter ref="A1:J20" xr:uid="{EA14FFEB-22C8-4B37-B805-3E79E719FB02}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1446,34 +1492,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>9</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>3</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" outlineLevel="1">
@@ -1482,23 +1528,23 @@
         <v>#REF!</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>716008</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>111131</v>
       </c>
       <c r="F2" s="15">
-        <f>-sheet1!H2</f>
+        <f>-sheet1!I2</f>
         <v>-9</v>
       </c>
       <c r="G2" t="str">
-        <f>sheet1!D2 &amp; "_" &amp;sheet1!I2 &amp; "_" &amp;sheet1!A2</f>
+        <f>sheet1!D2 &amp; "_" &amp;sheet1!J2 &amp; "_" &amp;sheet1!A2</f>
         <v>Town_A, State_I 10001_170_SAMCO_1</v>
       </c>
       <c r="I2" s="15">
@@ -1506,7 +1552,7 @@
         <v>-9</v>
       </c>
       <c r="J2" t="e">
-        <f xml:space="preserve"> sheet1!F2 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G2</f>
+        <f xml:space="preserve"> sheet1!G2 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H2</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1516,23 +1562,23 @@
         <v>#REF!</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>716008</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>111131</v>
       </c>
       <c r="F3" s="15">
-        <f>-sheet1!H3</f>
+        <f>-sheet1!I3</f>
         <v>-59</v>
       </c>
       <c r="G3" t="str">
-        <f>sheet1!D3 &amp; "_" &amp;sheet1!I3 &amp; "_" &amp;sheet1!A3</f>
+        <f>sheet1!D3 &amp; "_" &amp;sheet1!J3 &amp; "_" &amp;sheet1!A3</f>
         <v>Town_A, State_I 10001_941_SAMCO_1</v>
       </c>
       <c r="I3" s="15">
@@ -1540,7 +1586,7 @@
         <v>-59</v>
       </c>
       <c r="J3" t="e">
-        <f xml:space="preserve"> sheet1!F3 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G3</f>
+        <f xml:space="preserve"> sheet1!G3 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H3</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1550,23 +1596,23 @@
         <v>#REF!</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>716008</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>111131</v>
       </c>
       <c r="F4" s="15">
-        <f>-sheet1!H4</f>
+        <f>-sheet1!I4</f>
         <v>-39</v>
       </c>
       <c r="G4" t="str">
-        <f>sheet1!D4 &amp; "_" &amp;sheet1!I4 &amp; "_" &amp;sheet1!A4</f>
+        <f>sheet1!D4 &amp; "_" &amp;sheet1!J4 &amp; "_" &amp;sheet1!A4</f>
         <v>Town_A, State_I 10001_193_SAMCO_1</v>
       </c>
       <c r="I4" s="15">
@@ -1574,7 +1620,7 @@
         <v>-39</v>
       </c>
       <c r="J4" t="e">
-        <f xml:space="preserve"> sheet1!F4 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G4</f>
+        <f xml:space="preserve"> sheet1!G4 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H4</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1584,23 +1630,23 @@
         <v>#REF!</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>716008</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>111131</v>
       </c>
       <c r="F5" s="15">
-        <f>-sheet1!H5</f>
+        <f>-sheet1!I5</f>
         <v>-13</v>
       </c>
       <c r="G5" t="str">
-        <f>sheet1!D5 &amp; "_" &amp;sheet1!I5 &amp; "_" &amp;sheet1!A5</f>
+        <f>sheet1!D5 &amp; "_" &amp;sheet1!J5 &amp; "_" &amp;sheet1!A5</f>
         <v>Town_A, State_I 10001_526_SAMCO_1</v>
       </c>
       <c r="I5" s="15">
@@ -1608,7 +1654,7 @@
         <v>-13</v>
       </c>
       <c r="J5" t="e">
-        <f xml:space="preserve"> sheet1!F5 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G5</f>
+        <f xml:space="preserve"> sheet1!G5 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H5</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1618,23 +1664,23 @@
         <v>#REF!</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>716008</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>111131</v>
       </c>
       <c r="F6" s="15">
-        <f>-sheet1!H6</f>
+        <f>-sheet1!I6</f>
         <v>-71</v>
       </c>
       <c r="G6" t="str">
-        <f>sheet1!D6 &amp; "_" &amp;sheet1!I6 &amp; "_" &amp;sheet1!A6</f>
+        <f>sheet1!D6 &amp; "_" &amp;sheet1!J6 &amp; "_" &amp;sheet1!A6</f>
         <v>Town_A, State_I 10001_695_SAMCO_1</v>
       </c>
       <c r="I6" s="15">
@@ -1642,7 +1688,7 @@
         <v>-71</v>
       </c>
       <c r="J6" t="e">
-        <f xml:space="preserve"> sheet1!F6 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G6</f>
+        <f xml:space="preserve"> sheet1!G6 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H6</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1652,23 +1698,23 @@
         <v>#REF!</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>716008</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>111131</v>
       </c>
       <c r="F7" s="15">
-        <f>-sheet1!H7</f>
+        <f>-sheet1!I7</f>
         <v>-8</v>
       </c>
       <c r="G7" t="str">
-        <f>sheet1!D7 &amp; "_" &amp;sheet1!I7 &amp; "_" &amp;sheet1!A7</f>
+        <f>sheet1!D7 &amp; "_" &amp;sheet1!J7 &amp; "_" &amp;sheet1!A7</f>
         <v>Town_A, State_I 10001_632_SAMCO_1</v>
       </c>
       <c r="I7" s="15">
@@ -1676,7 +1722,7 @@
         <v>-8</v>
       </c>
       <c r="J7" t="e">
-        <f xml:space="preserve"> sheet1!F7 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G7</f>
+        <f xml:space="preserve"> sheet1!G7 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H7</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1686,23 +1732,23 @@
         <v>#REF!</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>716008</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>111131</v>
       </c>
       <c r="F8" s="15">
-        <f>-sheet1!H8</f>
+        <f>-sheet1!I8</f>
         <v>-69</v>
       </c>
       <c r="G8" t="str">
-        <f>sheet1!D8 &amp; "_" &amp;sheet1!I8 &amp; "_" &amp;sheet1!A8</f>
+        <f>sheet1!D8 &amp; "_" &amp;sheet1!J8 &amp; "_" &amp;sheet1!A8</f>
         <v>Town_A, State_I 10001_479_SAMCO_1</v>
       </c>
       <c r="I8" s="15">
@@ -1710,7 +1756,7 @@
         <v>-69</v>
       </c>
       <c r="J8" t="e">
-        <f xml:space="preserve"> sheet1!F8 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G8</f>
+        <f xml:space="preserve"> sheet1!G8 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H8</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1720,23 +1766,23 @@
         <v>#REF!</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>716008</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9">
         <v>111131</v>
       </c>
       <c r="F9" s="15">
-        <f>-sheet1!H9</f>
+        <f>-sheet1!I9</f>
         <v>-35</v>
       </c>
       <c r="G9" t="str">
-        <f>sheet1!D9 &amp; "_" &amp;sheet1!I9 &amp; "_" &amp;sheet1!A9</f>
+        <f>sheet1!D9 &amp; "_" &amp;sheet1!J9 &amp; "_" &amp;sheet1!A9</f>
         <v>Town_A, State_I 10001_173_SAMCO_1</v>
       </c>
       <c r="I9" s="15">
@@ -1744,7 +1790,7 @@
         <v>-35</v>
       </c>
       <c r="J9" t="e">
-        <f xml:space="preserve"> sheet1!F9 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G9</f>
+        <f xml:space="preserve"> sheet1!G9 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H9</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1754,23 +1800,23 @@
         <v>#REF!</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>716008</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <v>111131</v>
       </c>
       <c r="F10" s="15">
-        <f>-sheet1!H10</f>
+        <f>-sheet1!I10</f>
         <v>-73</v>
       </c>
       <c r="G10" t="str">
-        <f>sheet1!D10 &amp; "_" &amp;sheet1!I10 &amp; "_" &amp;sheet1!A10</f>
+        <f>sheet1!D10 &amp; "_" &amp;sheet1!J10 &amp; "_" &amp;sheet1!A10</f>
         <v>Town_A, State_I 10001_251_SAMCO_1</v>
       </c>
       <c r="I10" s="15">
@@ -1778,7 +1824,7 @@
         <v>-73</v>
       </c>
       <c r="J10" t="e">
-        <f xml:space="preserve"> sheet1!F10 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G10</f>
+        <f xml:space="preserve"> sheet1!G10 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H10</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1788,23 +1834,23 @@
         <v>#REF!</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>716008</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <v>111131</v>
       </c>
       <c r="F11" s="15">
-        <f>-sheet1!H11</f>
+        <f>-sheet1!I11</f>
         <v>-23</v>
       </c>
       <c r="G11" t="str">
-        <f>sheet1!D11 &amp; "_" &amp;sheet1!I11 &amp; "_" &amp;sheet1!A11</f>
+        <f>sheet1!D11 &amp; "_" &amp;sheet1!J11 &amp; "_" &amp;sheet1!A11</f>
         <v>Town_A, State_I 10001_154_SAMCO_1</v>
       </c>
       <c r="I11" s="15">
@@ -1812,7 +1858,7 @@
         <v>-23</v>
       </c>
       <c r="J11" t="e">
-        <f xml:space="preserve"> sheet1!F11 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G11</f>
+        <f xml:space="preserve"> sheet1!G11 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H11</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1822,23 +1868,23 @@
         <v>#REF!</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>716008</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>111131</v>
       </c>
       <c r="F12" s="15">
-        <f>-sheet1!H12</f>
+        <f>-sheet1!I12</f>
         <v>-13</v>
       </c>
       <c r="G12" t="str">
-        <f>sheet1!D12 &amp; "_" &amp;sheet1!I12 &amp; "_" &amp;sheet1!A12</f>
+        <f>sheet1!D12 &amp; "_" &amp;sheet1!J12 &amp; "_" &amp;sheet1!A12</f>
         <v>Town_A, State_I 10001_598_SAMCO_1</v>
       </c>
       <c r="I12" s="15">
@@ -1846,7 +1892,7 @@
         <v>-13</v>
       </c>
       <c r="J12" t="e">
-        <f xml:space="preserve"> sheet1!F12 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G12</f>
+        <f xml:space="preserve"> sheet1!G12 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H12</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1856,23 +1902,23 @@
         <v>#REF!</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>716008</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13">
         <v>111131</v>
       </c>
       <c r="F13" s="15">
-        <f>-sheet1!H13</f>
+        <f>-sheet1!I13</f>
         <v>-67</v>
       </c>
       <c r="G13" t="str">
-        <f>sheet1!D13 &amp; "_" &amp;sheet1!I13 &amp; "_" &amp;sheet1!A13</f>
+        <f>sheet1!D13 &amp; "_" &amp;sheet1!J13 &amp; "_" &amp;sheet1!A13</f>
         <v>Town_A, State_I 10001_587_SAMCO_1</v>
       </c>
       <c r="I13" s="15">
@@ -1880,7 +1926,7 @@
         <v>-67</v>
       </c>
       <c r="J13" t="e">
-        <f xml:space="preserve"> sheet1!F13 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G13</f>
+        <f xml:space="preserve"> sheet1!G13 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H13</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1890,23 +1936,23 @@
         <v>#REF!</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>716008</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <v>111131</v>
       </c>
       <c r="F14" s="15">
-        <f>-sheet1!H14</f>
+        <f>-sheet1!I14</f>
         <v>-70</v>
       </c>
       <c r="G14" t="str">
-        <f>sheet1!D14 &amp; "_" &amp;sheet1!I14 &amp; "_" &amp;sheet1!A14</f>
+        <f>sheet1!D14 &amp; "_" &amp;sheet1!J14 &amp; "_" &amp;sheet1!A14</f>
         <v>Town_A, State_I 10001_63_SAMCO_1</v>
       </c>
       <c r="I14" s="15">
@@ -1914,7 +1960,7 @@
         <v>-70</v>
       </c>
       <c r="J14" t="e">
-        <f xml:space="preserve"> sheet1!F14 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G14</f>
+        <f xml:space="preserve"> sheet1!G14 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H14</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1924,23 +1970,23 @@
         <v>#REF!</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>716008</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <v>111131</v>
       </c>
       <c r="F15" s="15">
-        <f>-sheet1!H15</f>
+        <f>-sheet1!I15</f>
         <v>-56</v>
       </c>
       <c r="G15" t="str">
-        <f>sheet1!D15 &amp; "_" &amp;sheet1!I15 &amp; "_" &amp;sheet1!A15</f>
+        <f>sheet1!D15 &amp; "_" &amp;sheet1!J15 &amp; "_" &amp;sheet1!A15</f>
         <v>Town_A, State_I 10001_639_SAMCO_1</v>
       </c>
       <c r="I15" s="15">
@@ -1948,7 +1994,7 @@
         <v>-56</v>
       </c>
       <c r="J15" t="e">
-        <f xml:space="preserve"> sheet1!F15 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G15</f>
+        <f xml:space="preserve"> sheet1!G15 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H15</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1958,23 +2004,23 @@
         <v>#REF!</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16">
         <v>716008</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>111131</v>
       </c>
       <c r="F16" s="15">
-        <f>-sheet1!H16</f>
+        <f>-sheet1!I16</f>
         <v>-12</v>
       </c>
       <c r="G16" t="str">
-        <f>sheet1!D16 &amp; "_" &amp;sheet1!I16 &amp; "_" &amp;sheet1!A16</f>
+        <f>sheet1!D16 &amp; "_" &amp;sheet1!J16 &amp; "_" &amp;sheet1!A16</f>
         <v>Town_A, State_I 10001_287_SAMCO_1</v>
       </c>
       <c r="I16" s="15">
@@ -1982,7 +2028,7 @@
         <v>-12</v>
       </c>
       <c r="J16" t="e">
-        <f xml:space="preserve"> sheet1!F16 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G16</f>
+        <f xml:space="preserve"> sheet1!G16 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H16</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -1992,23 +2038,23 @@
         <v>#REF!</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>716008</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>111131</v>
       </c>
       <c r="F17" s="15">
-        <f>-sheet1!H17</f>
+        <f>-sheet1!I17</f>
         <v>-69</v>
       </c>
       <c r="G17" t="str">
-        <f>sheet1!D17 &amp; "_" &amp;sheet1!I17 &amp; "_" &amp;sheet1!A17</f>
+        <f>sheet1!D17 &amp; "_" &amp;sheet1!J17 &amp; "_" &amp;sheet1!A17</f>
         <v>City_B, State_II 20002_302_SAMCO_2</v>
       </c>
       <c r="I17" s="15">
@@ -2016,7 +2062,7 @@
         <v>-69</v>
       </c>
       <c r="J17" t="e">
-        <f xml:space="preserve"> sheet1!F17 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G17</f>
+        <f xml:space="preserve"> sheet1!G17 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H17</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -2026,23 +2072,23 @@
         <v>#REF!</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>716008</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18">
         <v>111131</v>
       </c>
       <c r="F18" s="15">
-        <f>-sheet1!H18</f>
+        <f>-sheet1!I18</f>
         <v>-59</v>
       </c>
       <c r="G18" t="str">
-        <f>sheet1!D18 &amp; "_" &amp;sheet1!I18 &amp; "_" &amp;sheet1!A18</f>
+        <f>sheet1!D18 &amp; "_" &amp;sheet1!J18 &amp; "_" &amp;sheet1!A18</f>
         <v>City_C, State_III 30003_598_SAMCO_3</v>
       </c>
       <c r="I18" s="15">
@@ -2050,7 +2096,7 @@
         <v>-59</v>
       </c>
       <c r="J18" t="e">
-        <f xml:space="preserve"> sheet1!F18 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G18</f>
+        <f xml:space="preserve"> sheet1!G18 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H18</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -2060,23 +2106,23 @@
         <v>#REF!</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>716008</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19">
         <v>111131</v>
       </c>
       <c r="F19" s="15">
-        <f>-sheet1!H19</f>
+        <f>-sheet1!I19</f>
         <v>-23</v>
       </c>
       <c r="G19" t="str">
-        <f>sheet1!D19 &amp; "_" &amp;sheet1!I19 &amp; "_" &amp;sheet1!A19</f>
+        <f>sheet1!D19 &amp; "_" &amp;sheet1!J19 &amp; "_" &amp;sheet1!A19</f>
         <v>City_C, State_III 30003_463_SAMCO_3</v>
       </c>
       <c r="I19" s="15">
@@ -2084,7 +2130,7 @@
         <v>-23</v>
       </c>
       <c r="J19" t="e">
-        <f xml:space="preserve"> sheet1!F19 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G19</f>
+        <f xml:space="preserve"> sheet1!G19 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H19</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -2094,23 +2140,23 @@
         <v>#REF!</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>716009</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20">
         <v>111132</v>
       </c>
       <c r="F20" s="15">
-        <f>-sheet1!H20</f>
+        <f>-sheet1!I20</f>
         <v>-12</v>
       </c>
       <c r="G20" t="str">
-        <f>sheet1!D20 &amp; "_" &amp;sheet1!I20 &amp; "_" &amp;sheet1!A20</f>
+        <f>sheet1!D20 &amp; "_" &amp;sheet1!J20 &amp; "_" &amp;sheet1!A20</f>
         <v>City_C, State_III 30003_552_SAMCO_4</v>
       </c>
       <c r="I20" s="15">
@@ -2118,7 +2164,7 @@
         <v>-12</v>
       </c>
       <c r="J20" t="e">
-        <f xml:space="preserve"> sheet1!F20 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!G20</f>
+        <f xml:space="preserve"> sheet1!G20 &amp; "_" &amp; TEXT(sheet1!#REF!, "yyyymmdd") &amp; "_" &amp; sheet1!H20</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -2135,26 +2181,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cd7d8a8-4b84-4496-81b2-febcb680d7a6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="43d16329-3cf5-479a-9c03-b010a2369539" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100084E56D996A333499A63E7192D2DB564" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="071b7c44737a424e87a5adf4298b85a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9cd7d8a8-4b84-4496-81b2-febcb680d7a6" xmlns:ns3="43d16329-3cf5-479a-9c03-b010a2369539" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dedc65b3b6b20582fbd99b295097e86c" ns2:_="" ns3:_="">
     <xsd:import namespace="9cd7d8a8-4b84-4496-81b2-febcb680d7a6"/>
@@ -2361,26 +2387,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EAA25C6-E2F9-4C86-9EAE-6C3D08C02183}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C549155B-9936-4639-8BC0-A9AD07745483}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9cd7d8a8-4b84-4496-81b2-febcb680d7a6"/>
-    <ds:schemaRef ds:uri="43d16329-3cf5-479a-9c03-b010a2369539"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cd7d8a8-4b84-4496-81b2-febcb680d7a6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="43d16329-3cf5-479a-9c03-b010a2369539" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E5158AB-8FAE-4B2A-9A71-6007E8520FDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2397,4 +2424,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EAA25C6-E2F9-4C86-9EAE-6C3D08C02183}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C549155B-9936-4639-8BC0-A9AD07745483}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9cd7d8a8-4b84-4496-81b2-febcb680d7a6"/>
+    <ds:schemaRef ds:uri="43d16329-3cf5-479a-9c03-b010a2369539"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add comments and change template & sample data
- Add comments to the jupyter notebook
- Change the template
- Change the sample data format
</commit_message>
<xml_diff>
--- a/inv_info_sample.xlsx
+++ b/inv_info_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ningchuanpeng/Documents/GitHub/invoice-automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7E8363-521D-7942-86F1-9B3FFCA6AAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC308EB-A647-6D47-84DB-04725D0BF50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16340" xr2:uid="{F3C95119-47EE-434B-ACFE-389BE8C7694A}"/>
   </bookViews>
@@ -45,193 +45,194 @@
     <t>Amount</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Posting Date</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>Account No.</t>
+  </si>
+  <si>
+    <t>Bal. Account Type</t>
+  </si>
+  <si>
+    <t>Bal. Account No.</t>
+  </si>
+  <si>
+    <t>Currency Code</t>
+  </si>
+  <si>
+    <t>Amount ($)</t>
+  </si>
+  <si>
+    <t>G/L Account</t>
+  </si>
+  <si>
+    <t>Bank Account</t>
+  </si>
+  <si>
+    <t>Customer Address1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer Address2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Payment Terms</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAMCO_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAMCO_2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAMCO_3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAMCO_4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Detail</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Price</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quantity</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>123 ABC St.</t>
+  </si>
+  <si>
+    <t>123 ABC St.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit 1, 456 Ave.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Town_A, State_I 10001</t>
+  </si>
+  <si>
+    <t>Town_A, State_I 10001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>City_B, State_II 20002</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>City_C, State_III 30003</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apt. C, 789 St.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product 1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product 2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product 3</t>
+  </si>
+  <si>
+    <t>Product 4</t>
+  </si>
+  <si>
+    <t>Product 5</t>
+  </si>
+  <si>
+    <t>Product 6</t>
+  </si>
+  <si>
+    <t>Product 7</t>
+  </si>
+  <si>
+    <t>Product 8</t>
+  </si>
+  <si>
+    <t>Product 9</t>
+  </si>
+  <si>
+    <t>Product 10</t>
+  </si>
+  <si>
+    <t>Product 11</t>
+  </si>
+  <si>
+    <t>Product 12</t>
+  </si>
+  <si>
+    <t>Product 13</t>
+  </si>
+  <si>
+    <t>Product 14</t>
+  </si>
+  <si>
+    <t>Product 15</t>
+  </si>
+  <si>
+    <t>Product 7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product 10</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product 15</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invoice No.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Customer</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Posting Date</t>
-  </si>
-  <si>
-    <t>Account Type</t>
-  </si>
-  <si>
-    <t>Account No.</t>
-  </si>
-  <si>
-    <t>Bal. Account Type</t>
-  </si>
-  <si>
-    <t>Bal. Account No.</t>
-  </si>
-  <si>
-    <t>Currency Code</t>
-  </si>
-  <si>
-    <t>Amount ($)</t>
-  </si>
-  <si>
-    <t>G/L Account</t>
-  </si>
-  <si>
-    <t>Bank Account</t>
-  </si>
-  <si>
-    <t>Customer Address1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Customer Address2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Customer A</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Customer B</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Customer C</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Payment Terms</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAMCO_1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAMCO_2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAMCO_3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAMCO_4</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Detail</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit Price</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quantity</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>123 ABC St.</t>
-  </si>
-  <si>
-    <t>123 ABC St.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit 1, 456 Ave.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Town_A, State_I 10001</t>
-  </si>
-  <si>
-    <t>Town_A, State_I 10001</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>City_B, State_II 20002</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>City_C, State_III 30003</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apt. C, 789 St.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product 1</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product 2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product 3</t>
-  </si>
-  <si>
-    <t>Product 4</t>
-  </si>
-  <si>
-    <t>Product 5</t>
-  </si>
-  <si>
-    <t>Product 6</t>
-  </si>
-  <si>
-    <t>Product 7</t>
-  </si>
-  <si>
-    <t>Product 8</t>
-  </si>
-  <si>
-    <t>Product 9</t>
-  </si>
-  <si>
-    <t>Product 10</t>
-  </si>
-  <si>
-    <t>Product 11</t>
-  </si>
-  <si>
-    <t>Product 12</t>
-  </si>
-  <si>
-    <t>Product 13</t>
-  </si>
-  <si>
-    <t>Product 14</t>
-  </si>
-  <si>
-    <t>Product 15</t>
-  </si>
-  <si>
-    <t>Product 7</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product 10</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Product 15</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invoice Date</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Invoice No.</t>
-    <phoneticPr fontId="5" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -258,13 +259,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -283,6 +277,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -293,12 +293,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -379,69 +379,65 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -781,7 +777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA14FFEB-22C8-4B37-B805-3E79E719FB02}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -792,672 +790,672 @@
     <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="17" thickBot="1">
+      <c r="A1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16">
-      <c r="A2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="17">
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="12">
         <v>45657</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4">
         <v>30</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="5" t="str">
+      <c r="G2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="str">
         <f>G2 &amp; " details"</f>
         <v>Product 1 details</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="3">
         <v>9</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="4">
         <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16">
-      <c r="A3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="12">
         <v>45657</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="5" t="str">
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="str">
         <f t="shared" ref="H3:H20" si="0">G3 &amp; " details"</f>
         <v>Product 2 details</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="3">
         <v>59</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="4">
         <v>941</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16">
-      <c r="A4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F4" s="4">
         <v>30</v>
       </c>
-      <c r="E4" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F4" s="7">
-        <v>30</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="5" t="str">
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 3 details</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <v>39</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="4">
         <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F5" s="4">
         <v>30</v>
       </c>
-      <c r="E5" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F5" s="7">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="5" t="str">
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 4 details</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <v>13</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <v>526</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16">
-      <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F6" s="4">
         <v>30</v>
       </c>
-      <c r="E6" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F6" s="7">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="5" t="str">
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 5 details</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <v>71</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <v>695</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16">
-      <c r="A7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F7" s="4">
         <v>30</v>
       </c>
-      <c r="E7" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F7" s="7">
-        <v>30</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="5" t="str">
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 6 details</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="3">
         <v>8</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <v>632</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F8" s="4">
         <v>30</v>
       </c>
-      <c r="E8" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F8" s="7">
-        <v>30</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="5" t="str">
+      <c r="G8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 7 details</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <v>69</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="4">
         <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16">
-      <c r="A9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F9" s="4">
         <v>30</v>
       </c>
-      <c r="E9" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F9" s="7">
-        <v>30</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="5" t="str">
+      <c r="G9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 8 details</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="3">
         <v>35</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="4">
         <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16">
-      <c r="A10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F10" s="4">
         <v>30</v>
       </c>
-      <c r="E10" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F10" s="7">
-        <v>30</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="5" t="str">
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 9 details</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <v>73</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="4">
         <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16">
-      <c r="A11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F11" s="4">
         <v>30</v>
       </c>
-      <c r="E11" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F11" s="7">
-        <v>30</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="5" t="str">
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 10 details</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="3">
         <v>23</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="4">
         <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16">
-      <c r="A12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F12" s="4">
         <v>30</v>
       </c>
-      <c r="E12" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F12" s="7">
-        <v>30</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="5" t="str">
+      <c r="G12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 11 details</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <v>13</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="4">
         <v>598</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16">
-      <c r="A13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F13" s="4">
         <v>30</v>
       </c>
-      <c r="E13" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F13" s="7">
-        <v>30</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="5" t="str">
+      <c r="G13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 12 details</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="3">
         <v>67</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="4">
         <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16">
-      <c r="A14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F14" s="4">
         <v>30</v>
       </c>
-      <c r="E14" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F14" s="7">
-        <v>30</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="5" t="str">
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 13 details</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="3">
         <v>70</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="4">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16">
-      <c r="A15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F15" s="4">
         <v>30</v>
       </c>
-      <c r="E15" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F15" s="7">
-        <v>30</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="5" t="str">
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 14 details</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="3">
         <v>56</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="4">
         <v>639</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16">
-      <c r="A16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="12">
+        <v>45657</v>
+      </c>
+      <c r="F16" s="4">
         <v>30</v>
       </c>
-      <c r="E16" s="17">
-        <v>45657</v>
-      </c>
-      <c r="F16" s="7">
-        <v>30</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="5" t="str">
+      <c r="G16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 15 details</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="3">
         <v>12</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="4">
         <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16">
-      <c r="A17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="17">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="12">
         <v>45668</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>90</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="5" t="str">
+      <c r="G17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 7 details</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="8">
         <v>69</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="4">
         <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16">
-      <c r="A18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="17">
+      <c r="D18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="12">
         <v>45704</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="4">
         <v>60</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="5" t="str">
+      <c r="G18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 2 details</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="8">
         <v>59</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="4">
         <v>598</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="17">
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="12">
         <v>45704</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="4">
         <v>60</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H19" s="5" t="str">
+      <c r="G19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 10 details</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="8">
         <v>23</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="4">
         <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16">
-      <c r="A20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="17">
+      <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="12">
         <v>45737</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="4">
         <v>60</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="5" t="str">
+      <c r="G20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Product 15 details</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="8">
         <v>12</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="4">
         <v>552</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J20" xr:uid="{EA14FFEB-22C8-4B37-B805-3E79E719FB02}"/>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -1491,55 +1489,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="A2" s="10" t="e">
+        <f>sheet1!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A2" s="14" t="e">
-        <f>sheet1!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2">
         <v>716008</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>111131</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="11">
         <f>-sheet1!I2</f>
         <v>-9</v>
       </c>
@@ -1547,7 +1545,7 @@
         <f>sheet1!D2 &amp; "_" &amp;sheet1!J2 &amp; "_" &amp;sheet1!A2</f>
         <v>Town_A, State_I 10001_170_SAMCO_1</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="11">
         <f>F2</f>
         <v>-9</v>
       </c>
@@ -1557,23 +1555,23 @@
       </c>
     </row>
     <row r="3" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A3" s="14" t="e">
+      <c r="A3" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>716008</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>111131</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="11">
         <f>-sheet1!I3</f>
         <v>-59</v>
       </c>
@@ -1581,7 +1579,7 @@
         <f>sheet1!D3 &amp; "_" &amp;sheet1!J3 &amp; "_" &amp;sheet1!A3</f>
         <v>Town_A, State_I 10001_941_SAMCO_1</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f t="shared" ref="I3:I10" si="0">F3</f>
         <v>-59</v>
       </c>
@@ -1591,23 +1589,23 @@
       </c>
     </row>
     <row r="4" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A4" s="14" t="e">
+      <c r="A4" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>716008</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>111131</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="11">
         <f>-sheet1!I4</f>
         <v>-39</v>
       </c>
@@ -1615,7 +1613,7 @@
         <f>sheet1!D4 &amp; "_" &amp;sheet1!J4 &amp; "_" &amp;sheet1!A4</f>
         <v>Town_A, State_I 10001_193_SAMCO_1</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="11">
         <f t="shared" si="0"/>
         <v>-39</v>
       </c>
@@ -1625,23 +1623,23 @@
       </c>
     </row>
     <row r="5" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A5" s="14" t="e">
+      <c r="A5" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>716008</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>111131</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>-sheet1!I5</f>
         <v>-13</v>
       </c>
@@ -1649,7 +1647,7 @@
         <f>sheet1!D5 &amp; "_" &amp;sheet1!J5 &amp; "_" &amp;sheet1!A5</f>
         <v>Town_A, State_I 10001_526_SAMCO_1</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <f t="shared" si="0"/>
         <v>-13</v>
       </c>
@@ -1659,23 +1657,23 @@
       </c>
     </row>
     <row r="6" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A6" s="14" t="e">
+      <c r="A6" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>716008</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>111131</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="11">
         <f>-sheet1!I6</f>
         <v>-71</v>
       </c>
@@ -1683,7 +1681,7 @@
         <f>sheet1!D6 &amp; "_" &amp;sheet1!J6 &amp; "_" &amp;sheet1!A6</f>
         <v>Town_A, State_I 10001_695_SAMCO_1</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="11">
         <f t="shared" si="0"/>
         <v>-71</v>
       </c>
@@ -1693,23 +1691,23 @@
       </c>
     </row>
     <row r="7" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A7" s="14" t="e">
+      <c r="A7" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>716008</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>111131</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="11">
         <f>-sheet1!I7</f>
         <v>-8</v>
       </c>
@@ -1717,7 +1715,7 @@
         <f>sheet1!D7 &amp; "_" &amp;sheet1!J7 &amp; "_" &amp;sheet1!A7</f>
         <v>Town_A, State_I 10001_632_SAMCO_1</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="11">
         <f t="shared" si="0"/>
         <v>-8</v>
       </c>
@@ -1727,23 +1725,23 @@
       </c>
     </row>
     <row r="8" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A8" s="14" t="e">
+      <c r="A8" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>716008</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>111131</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="11">
         <f>-sheet1!I8</f>
         <v>-69</v>
       </c>
@@ -1751,7 +1749,7 @@
         <f>sheet1!D8 &amp; "_" &amp;sheet1!J8 &amp; "_" &amp;sheet1!A8</f>
         <v>Town_A, State_I 10001_479_SAMCO_1</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="11">
         <f t="shared" si="0"/>
         <v>-69</v>
       </c>
@@ -1761,23 +1759,23 @@
       </c>
     </row>
     <row r="9" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A9" s="14" t="e">
+      <c r="A9" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>716008</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>111131</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="11">
         <f>-sheet1!I9</f>
         <v>-35</v>
       </c>
@@ -1785,7 +1783,7 @@
         <f>sheet1!D9 &amp; "_" &amp;sheet1!J9 &amp; "_" &amp;sheet1!A9</f>
         <v>Town_A, State_I 10001_173_SAMCO_1</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="11">
         <f t="shared" si="0"/>
         <v>-35</v>
       </c>
@@ -1795,23 +1793,23 @@
       </c>
     </row>
     <row r="10" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A10" s="14" t="e">
+      <c r="A10" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>716008</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>111131</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="11">
         <f>-sheet1!I10</f>
         <v>-73</v>
       </c>
@@ -1819,7 +1817,7 @@
         <f>sheet1!D10 &amp; "_" &amp;sheet1!J10 &amp; "_" &amp;sheet1!A10</f>
         <v>Town_A, State_I 10001_251_SAMCO_1</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="11">
         <f t="shared" si="0"/>
         <v>-73</v>
       </c>
@@ -1829,23 +1827,23 @@
       </c>
     </row>
     <row r="11" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A11" s="14" t="e">
+      <c r="A11" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>716008</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>111131</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="11">
         <f>-sheet1!I11</f>
         <v>-23</v>
       </c>
@@ -1853,7 +1851,7 @@
         <f>sheet1!D11 &amp; "_" &amp;sheet1!J11 &amp; "_" &amp;sheet1!A11</f>
         <v>Town_A, State_I 10001_154_SAMCO_1</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="11">
         <f t="shared" ref="I11:I13" si="1">F11</f>
         <v>-23</v>
       </c>
@@ -1863,23 +1861,23 @@
       </c>
     </row>
     <row r="12" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A12" s="14" t="e">
+      <c r="A12" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>716008</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>111131</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="11">
         <f>-sheet1!I12</f>
         <v>-13</v>
       </c>
@@ -1887,7 +1885,7 @@
         <f>sheet1!D12 &amp; "_" &amp;sheet1!J12 &amp; "_" &amp;sheet1!A12</f>
         <v>Town_A, State_I 10001_598_SAMCO_1</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="11">
         <f t="shared" si="1"/>
         <v>-13</v>
       </c>
@@ -1897,23 +1895,23 @@
       </c>
     </row>
     <row r="13" spans="1:10" collapsed="1">
-      <c r="A13" s="14" t="e">
+      <c r="A13" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>716008</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>111131</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="11">
         <f>-sheet1!I13</f>
         <v>-67</v>
       </c>
@@ -1921,7 +1919,7 @@
         <f>sheet1!D13 &amp; "_" &amp;sheet1!J13 &amp; "_" &amp;sheet1!A13</f>
         <v>Town_A, State_I 10001_587_SAMCO_1</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="11">
         <f t="shared" si="1"/>
         <v>-67</v>
       </c>
@@ -1931,23 +1929,23 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="14" t="e">
+      <c r="A14" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>716008</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>111131</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="11">
         <f>-sheet1!I14</f>
         <v>-70</v>
       </c>
@@ -1955,7 +1953,7 @@
         <f>sheet1!D14 &amp; "_" &amp;sheet1!J14 &amp; "_" &amp;sheet1!A14</f>
         <v>Town_A, State_I 10001_63_SAMCO_1</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="11">
         <f t="shared" ref="I14:I16" si="2">F14</f>
         <v>-70</v>
       </c>
@@ -1965,23 +1963,23 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="14" t="e">
+      <c r="A15" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>716008</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15">
         <v>111131</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="11">
         <f>-sheet1!I15</f>
         <v>-56</v>
       </c>
@@ -1989,7 +1987,7 @@
         <f>sheet1!D15 &amp; "_" &amp;sheet1!J15 &amp; "_" &amp;sheet1!A15</f>
         <v>Town_A, State_I 10001_639_SAMCO_1</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="11">
         <f t="shared" si="2"/>
         <v>-56</v>
       </c>
@@ -1999,23 +1997,23 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="14" t="e">
+      <c r="A16" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>716008</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>111131</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="11">
         <f>-sheet1!I16</f>
         <v>-12</v>
       </c>
@@ -2023,7 +2021,7 @@
         <f>sheet1!D16 &amp; "_" &amp;sheet1!J16 &amp; "_" &amp;sheet1!A16</f>
         <v>Town_A, State_I 10001_287_SAMCO_1</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="11">
         <f t="shared" si="2"/>
         <v>-12</v>
       </c>
@@ -2033,23 +2031,23 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="14" t="e">
+      <c r="A17" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>716008</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17">
         <v>111131</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="11">
         <f>-sheet1!I17</f>
         <v>-69</v>
       </c>
@@ -2057,7 +2055,7 @@
         <f>sheet1!D17 &amp; "_" &amp;sheet1!J17 &amp; "_" &amp;sheet1!A17</f>
         <v>City_B, State_II 20002_302_SAMCO_2</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="11">
         <f t="shared" ref="I17:I19" si="3">F17</f>
         <v>-69</v>
       </c>
@@ -2067,23 +2065,23 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="14" t="e">
+      <c r="A18" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>716008</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18">
         <v>111131</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="11">
         <f>-sheet1!I18</f>
         <v>-59</v>
       </c>
@@ -2091,7 +2089,7 @@
         <f>sheet1!D18 &amp; "_" &amp;sheet1!J18 &amp; "_" &amp;sheet1!A18</f>
         <v>City_C, State_III 30003_598_SAMCO_3</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="11">
         <f t="shared" si="3"/>
         <v>-59</v>
       </c>
@@ -2101,23 +2099,23 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="14" t="e">
+      <c r="A19" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>716008</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <v>111131</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="11">
         <f>-sheet1!I19</f>
         <v>-23</v>
       </c>
@@ -2125,7 +2123,7 @@
         <f>sheet1!D19 &amp; "_" &amp;sheet1!J19 &amp; "_" &amp;sheet1!A19</f>
         <v>City_C, State_III 30003_463_SAMCO_3</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="11">
         <f t="shared" si="3"/>
         <v>-23</v>
       </c>
@@ -2135,23 +2133,23 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="14" t="e">
+      <c r="A20" s="10" t="e">
         <f>sheet1!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>716009</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>111132</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="11">
         <f>-sheet1!I20</f>
         <v>-12</v>
       </c>
@@ -2159,7 +2157,7 @@
         <f>sheet1!D20 &amp; "_" &amp;sheet1!J20 &amp; "_" &amp;sheet1!A20</f>
         <v>City_C, State_III 30003_552_SAMCO_4</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="11">
         <f t="shared" ref="I20" si="4">F20</f>
         <v>-12</v>
       </c>
@@ -2169,7 +2167,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2388,15 +2386,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9cd7d8a8-4b84-4496-81b2-febcb680d7a6">
@@ -2405,6 +2394,15 @@
     <TaxCatchAll xmlns="43d16329-3cf5-479a-9c03-b010a2369539" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2427,14 +2425,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EAA25C6-E2F9-4C86-9EAE-6C3D08C02183}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C549155B-9936-4639-8BC0-A9AD07745483}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2443,4 +2433,12 @@
     <ds:schemaRef ds:uri="43d16329-3cf5-479a-9c03-b010a2369539"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EAA25C6-E2F9-4C86-9EAE-6C3D08C02183}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>